<commit_message>
Mainly: Comment out developer options
</commit_message>
<xml_diff>
--- a/input/Dash_LCOE_ConfigurationV3.xlsx
+++ b/input/Dash_LCOE_ConfigurationV3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Florian\PycharmProjects\LCOEcalc\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C63974BD-6748-4737-9FAC-4F93E7CC8BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93A8F2A-EAC3-4E24-9B09-3A40F8768E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Systems" sheetId="1" r:id="rId1"/>
@@ -1506,8 +1506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5708E7F0-2DE7-4611-91D4-02BADD085AA2}">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1536,13 +1536,13 @@
         <v>42</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -1643,10 +1643,10 @@
         <v>15</v>
       </c>
       <c r="G5" s="5">
+        <v>10</v>
+      </c>
+      <c r="H5" s="5">
         <v>15</v>
-      </c>
-      <c r="H5" s="5">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1669,10 +1669,10 @@
         <v>10</v>
       </c>
       <c r="G6" s="5">
+        <v>8</v>
+      </c>
+      <c r="H6" s="5">
         <v>10</v>
-      </c>
-      <c r="H6" s="5">
-        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -1695,10 +1695,10 @@
         <v>20</v>
       </c>
       <c r="G7" s="5">
+        <v>12</v>
+      </c>
+      <c r="H7" s="5">
         <v>20</v>
-      </c>
-      <c r="H7" s="5">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1721,10 +1721,10 @@
         <v>6000</v>
       </c>
       <c r="G8" s="5">
+        <v>750</v>
+      </c>
+      <c r="H8" s="5">
         <v>6000</v>
-      </c>
-      <c r="H8" s="5">
-        <v>750</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -1747,10 +1747,10 @@
         <v>4500</v>
       </c>
       <c r="G9" s="5">
+        <v>700</v>
+      </c>
+      <c r="H9" s="5">
         <v>4500</v>
-      </c>
-      <c r="H9" s="5">
-        <v>700</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -1773,10 +1773,10 @@
         <v>7000</v>
       </c>
       <c r="G10" s="5">
+        <v>800</v>
+      </c>
+      <c r="H10" s="5">
         <v>7000</v>
-      </c>
-      <c r="H10" s="5">
-        <v>800</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -2738,7 +2738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C16DF341-8C1A-4D19-88F8-FE2D2A0FBA8F}">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>

</xml_diff>